<commit_message>
corrected nivar and bulbul
</commit_message>
<xml_diff>
--- a/dataproc/list_of_cyclones.xlsx
+++ b/dataproc/list_of_cyclones.xlsx
@@ -1,29 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20412"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2484CC43-2E7F-49D6-BF55-B1045A05FD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ren\forecast-diffmodels\dataproc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5494F137-A53E-4F5E-B04B-58C4C638C61D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -138,12 +130,6 @@
     <t>Category 3</t>
   </si>
   <si>
-    <t>05-11-2019</t>
-  </si>
-  <si>
-    <t>11-11-2019</t>
-  </si>
-  <si>
     <t>https://en.wikipedia.org/wiki/Cyclone_Matmo-Bulbul</t>
   </si>
   <si>
@@ -739,13 +725,19 @@
   </si>
   <si>
     <t>South West Indian Ocean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28-10-2019	</t>
+  </si>
+  <si>
+    <t>31-10-2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1215,23 +1207,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.26953125" customWidth="1"/>
+    <col min="2" max="2" width="30.81640625" customWidth="1"/>
+    <col min="3" max="3" width="32.81640625" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="5" max="5" width="26.1796875" customWidth="1"/>
+    <col min="6" max="6" width="14.26953125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="57" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1257,7 +1249,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1286,7 +1278,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1313,7 +1305,7 @@
       </c>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1342,7 +1334,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1369,7 +1361,7 @@
       </c>
       <c r="I5" s="10"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1398,7 +1390,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1415,19 +1407,19 @@
         <v>35</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1438,25 +1430,25 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1469,179 +1461,179 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>47</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="H11" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
         <v>35</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="2" t="s">
+      <c r="H14" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s">
         <v>35</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1651,163 +1643,163 @@
       <c r="G16" s="9"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
         <v>71</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>72</v>
-      </c>
-      <c r="C17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" t="s">
-        <v>74</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" t="s">
         <v>76</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" t="s">
-        <v>78</v>
       </c>
       <c r="E18" t="s">
         <v>35</v>
       </c>
       <c r="F18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G18" s="2" t="s">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="s">
         <v>80</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" t="s">
-        <v>83</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G19" s="2" t="s">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" t="s">
         <v>85</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="E20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" t="s">
+      <c r="G20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
         <v>71</v>
       </c>
-      <c r="B20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" t="s">
-        <v>87</v>
-      </c>
-      <c r="E20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="2" t="s">
+      <c r="D21" t="s">
         <v>89</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" t="s">
-        <v>91</v>
       </c>
       <c r="E21" t="s">
         <v>35</v>
       </c>
       <c r="F21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G21" s="2" t="s">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" t="s">
         <v>93</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="E22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="G22" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E22" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="2" t="s">
+      <c r="H22" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1817,215 +1809,215 @@
       <c r="G23" s="9"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" t="s">
         <v>99</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>100</v>
-      </c>
-      <c r="C24" t="s">
-        <v>101</v>
-      </c>
-      <c r="D24" t="s">
-        <v>102</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" t="s">
         <v>104</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="E25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="s">
+      <c r="G25" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" t="s">
         <v>99</v>
       </c>
-      <c r="B25" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" t="s">
-        <v>106</v>
-      </c>
-      <c r="E25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G25" s="2" t="s">
+      <c r="D26" t="s">
         <v>108</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="E26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" t="s">
+      <c r="G26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" t="s">
         <v>99</v>
       </c>
-      <c r="B26" t="s">
-        <v>100</v>
-      </c>
-      <c r="C26" t="s">
-        <v>101</v>
-      </c>
-      <c r="D26" t="s">
-        <v>110</v>
-      </c>
-      <c r="E26" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G26" s="2" t="s">
+      <c r="D27" t="s">
         <v>112</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="E27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" t="s">
+      <c r="G27" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" t="s">
         <v>99</v>
       </c>
-      <c r="B27" t="s">
-        <v>100</v>
-      </c>
-      <c r="C27" t="s">
-        <v>101</v>
-      </c>
-      <c r="D27" t="s">
-        <v>114</v>
-      </c>
-      <c r="E27" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G27" s="2" t="s">
+      <c r="D28" t="s">
         <v>116</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" t="s">
-        <v>99</v>
-      </c>
-      <c r="B28" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" t="s">
-        <v>101</v>
-      </c>
-      <c r="D28" t="s">
-        <v>118</v>
       </c>
       <c r="E28" t="s">
         <v>35</v>
       </c>
       <c r="F28" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G28" s="2" t="s">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" t="s">
         <v>120</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="E29" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" t="s">
+      <c r="G29" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" t="s">
         <v>99</v>
       </c>
-      <c r="B29" t="s">
-        <v>100</v>
-      </c>
-      <c r="C29" t="s">
-        <v>101</v>
-      </c>
-      <c r="D29" t="s">
-        <v>122</v>
-      </c>
-      <c r="E29" t="s">
-        <v>55</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G29" s="2" t="s">
+      <c r="D30" t="s">
         <v>124</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="E30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" t="s">
+      <c r="G30" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" t="s">
         <v>99</v>
       </c>
-      <c r="B30" t="s">
-        <v>100</v>
-      </c>
-      <c r="C30" t="s">
-        <v>101</v>
-      </c>
-      <c r="D30" t="s">
-        <v>126</v>
-      </c>
-      <c r="E30" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G30" s="2" t="s">
+      <c r="D31" t="s">
         <v>128</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" t="s">
-        <v>100</v>
-      </c>
-      <c r="C31" t="s">
-        <v>101</v>
-      </c>
-      <c r="D31" t="s">
-        <v>130</v>
       </c>
       <c r="E31" t="s">
         <v>35</v>
       </c>
       <c r="F31" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2035,293 +2027,293 @@
       <c r="G32" s="9"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" t="s">
         <v>134</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" t="s">
         <v>135</v>
-      </c>
-      <c r="C33" t="s">
-        <v>136</v>
-      </c>
-      <c r="D33" t="s">
-        <v>137</v>
       </c>
       <c r="E33" t="s">
         <v>12</v>
       </c>
       <c r="F33" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G33" s="2" t="s">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" t="s">
         <v>139</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="E34" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" t="s">
+      <c r="G34" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" t="s">
         <v>134</v>
       </c>
-      <c r="B34" t="s">
-        <v>135</v>
-      </c>
-      <c r="C34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D34" t="s">
-        <v>141</v>
-      </c>
-      <c r="E34" t="s">
-        <v>50</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G34" s="2" t="s">
+      <c r="D35" t="s">
         <v>143</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="E35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" t="s">
+      <c r="G35" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" t="s">
         <v>134</v>
       </c>
-      <c r="B35" t="s">
-        <v>135</v>
-      </c>
-      <c r="C35" t="s">
-        <v>136</v>
-      </c>
-      <c r="D35" t="s">
-        <v>145</v>
-      </c>
-      <c r="E35" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G35" s="2" t="s">
+      <c r="D36" t="s">
         <v>147</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" t="s">
-        <v>134</v>
-      </c>
-      <c r="B36" t="s">
-        <v>135</v>
-      </c>
-      <c r="C36" t="s">
-        <v>136</v>
-      </c>
-      <c r="D36" t="s">
-        <v>149</v>
       </c>
       <c r="E36" t="s">
         <v>35</v>
       </c>
       <c r="F36" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G36" s="2" t="s">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" t="s">
+        <v>133</v>
+      </c>
+      <c r="C37" t="s">
+        <v>134</v>
+      </c>
+      <c r="D37" t="s">
         <v>151</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" t="s">
-        <v>134</v>
-      </c>
-      <c r="B37" t="s">
-        <v>135</v>
-      </c>
-      <c r="C37" t="s">
-        <v>136</v>
-      </c>
-      <c r="D37" t="s">
-        <v>153</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
       </c>
       <c r="F37" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G37" s="2" t="s">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>132</v>
+      </c>
+      <c r="B38" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" t="s">
         <v>155</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="E38" t="s">
+        <v>48</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" t="s">
+      <c r="G38" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39" t="s">
+        <v>133</v>
+      </c>
+      <c r="C39" t="s">
         <v>134</v>
       </c>
-      <c r="B38" t="s">
-        <v>135</v>
-      </c>
-      <c r="C38" t="s">
-        <v>136</v>
-      </c>
-      <c r="D38" t="s">
-        <v>157</v>
-      </c>
-      <c r="E38" t="s">
-        <v>50</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="G38" s="2" t="s">
+      <c r="D39" t="s">
         <v>159</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" t="s">
-        <v>134</v>
-      </c>
-      <c r="B39" t="s">
-        <v>135</v>
-      </c>
-      <c r="C39" t="s">
-        <v>136</v>
-      </c>
-      <c r="D39" t="s">
-        <v>161</v>
       </c>
       <c r="E39" t="s">
         <v>35</v>
       </c>
       <c r="F39" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="G39" s="2" t="s">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B40" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" t="s">
+        <v>134</v>
+      </c>
+      <c r="D40" t="s">
         <v>163</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="E40" t="s">
+        <v>48</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" t="s">
+      <c r="G40" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>132</v>
+      </c>
+      <c r="B41" t="s">
+        <v>133</v>
+      </c>
+      <c r="C41" t="s">
         <v>134</v>
       </c>
-      <c r="B40" t="s">
-        <v>135</v>
-      </c>
-      <c r="C40" t="s">
-        <v>136</v>
-      </c>
-      <c r="D40" t="s">
-        <v>165</v>
-      </c>
-      <c r="E40" t="s">
-        <v>50</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="G40" s="2" t="s">
+      <c r="D41" t="s">
         <v>167</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="E41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" t="s">
+      <c r="G41" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>132</v>
+      </c>
+      <c r="B42" t="s">
+        <v>133</v>
+      </c>
+      <c r="C42" t="s">
         <v>134</v>
       </c>
-      <c r="B41" t="s">
-        <v>135</v>
-      </c>
-      <c r="C41" t="s">
-        <v>136</v>
-      </c>
-      <c r="D41" t="s">
-        <v>169</v>
-      </c>
-      <c r="E41" t="s">
-        <v>55</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="G41" s="2" t="s">
+      <c r="D42" t="s">
         <v>171</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="E42" t="s">
+        <v>48</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" t="s">
+      <c r="G42" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>132</v>
+      </c>
+      <c r="B43" t="s">
+        <v>133</v>
+      </c>
+      <c r="C43" t="s">
         <v>134</v>
       </c>
-      <c r="B42" t="s">
-        <v>135</v>
-      </c>
-      <c r="C42" t="s">
-        <v>136</v>
-      </c>
-      <c r="D42" t="s">
-        <v>173</v>
-      </c>
-      <c r="E42" t="s">
-        <v>50</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G42" s="2" t="s">
+      <c r="D43" t="s">
         <v>175</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" t="s">
-        <v>134</v>
-      </c>
-      <c r="B43" t="s">
-        <v>135</v>
-      </c>
-      <c r="C43" t="s">
-        <v>136</v>
-      </c>
-      <c r="D43" t="s">
-        <v>177</v>
       </c>
       <c r="E43" t="s">
         <v>35</v>
       </c>
       <c r="F43" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -2331,111 +2323,111 @@
       <c r="G44" s="9"/>
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
+        <v>179</v>
+      </c>
+      <c r="B45" t="s">
+        <v>180</v>
+      </c>
+      <c r="C45" t="s">
         <v>181</v>
       </c>
-      <c r="B45" t="s">
+      <c r="D45" t="s">
         <v>182</v>
       </c>
-      <c r="C45" t="s">
+      <c r="E45" t="s">
+        <v>48</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D45" t="s">
+      <c r="G45" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E45" t="s">
-        <v>50</v>
-      </c>
-      <c r="F45" s="2" t="s">
+      <c r="H45" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="G45" s="2" t="s">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46" t="s">
+        <v>180</v>
+      </c>
+      <c r="C46" t="s">
+        <v>181</v>
+      </c>
+      <c r="D46" t="s">
         <v>186</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="E46" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" t="s">
+      <c r="G46" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>179</v>
+      </c>
+      <c r="B47" t="s">
+        <v>180</v>
+      </c>
+      <c r="C47" t="s">
         <v>181</v>
       </c>
-      <c r="B46" t="s">
-        <v>182</v>
-      </c>
-      <c r="C46" t="s">
-        <v>183</v>
-      </c>
-      <c r="D46" t="s">
-        <v>188</v>
-      </c>
-      <c r="E46" t="s">
-        <v>50</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G46" s="2" t="s">
+      <c r="D47" t="s">
         <v>190</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="E47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" t="s">
+      <c r="G47" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" t="s">
         <v>181</v>
       </c>
-      <c r="B47" t="s">
-        <v>182</v>
-      </c>
-      <c r="C47" t="s">
-        <v>183</v>
-      </c>
-      <c r="D47" t="s">
-        <v>192</v>
-      </c>
-      <c r="E47" t="s">
-        <v>55</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="G47" s="2" t="s">
+      <c r="D48" t="s">
         <v>194</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="E48" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" t="s">
-        <v>181</v>
-      </c>
-      <c r="B48" t="s">
-        <v>182</v>
-      </c>
-      <c r="C48" t="s">
-        <v>183</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="G48" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E48" t="s">
-        <v>50</v>
-      </c>
-      <c r="F48" s="2" t="s">
+      <c r="H48" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="G48" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -2445,241 +2437,241 @@
       <c r="G49" s="9"/>
       <c r="H49" s="4"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>198</v>
+      </c>
+      <c r="B50" t="s">
+        <v>199</v>
+      </c>
+      <c r="C50" t="s">
+        <v>71</v>
+      </c>
+      <c r="D50" t="s">
         <v>200</v>
-      </c>
-      <c r="B50" t="s">
-        <v>201</v>
-      </c>
-      <c r="C50" t="s">
-        <v>73</v>
-      </c>
-      <c r="D50" t="s">
-        <v>202</v>
       </c>
       <c r="E50" t="s">
         <v>12</v>
       </c>
       <c r="F50" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>198</v>
+      </c>
+      <c r="B51" t="s">
+        <v>199</v>
+      </c>
+      <c r="C51" t="s">
+        <v>71</v>
+      </c>
+      <c r="D51" t="s">
         <v>203</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="H50" s="1" t="s">
+      <c r="E51" t="s">
+        <v>53</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" t="s">
-        <v>200</v>
-      </c>
-      <c r="B51" t="s">
-        <v>201</v>
-      </c>
-      <c r="C51" t="s">
-        <v>73</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="G51" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="H51" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E51" t="s">
-        <v>55</v>
-      </c>
-      <c r="F51" s="2" t="s">
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>198</v>
+      </c>
+      <c r="B52" t="s">
+        <v>199</v>
+      </c>
+      <c r="C52" t="s">
+        <v>71</v>
+      </c>
+      <c r="D52" t="s">
         <v>206</v>
       </c>
-      <c r="G51" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="H51" s="1" t="s">
+      <c r="E52" t="s">
+        <v>48</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" t="s">
-        <v>200</v>
-      </c>
-      <c r="B52" t="s">
-        <v>201</v>
-      </c>
-      <c r="C52" t="s">
-        <v>73</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="G52" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E52" t="s">
-        <v>50</v>
-      </c>
-      <c r="F52" s="2" t="s">
+      <c r="H52" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G52" s="2" t="s">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>198</v>
+      </c>
+      <c r="B53" t="s">
+        <v>199</v>
+      </c>
+      <c r="C53" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" t="s">
         <v>210</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" t="s">
-        <v>200</v>
-      </c>
-      <c r="B53" t="s">
-        <v>201</v>
-      </c>
-      <c r="C53" t="s">
-        <v>73</v>
-      </c>
-      <c r="D53" t="s">
-        <v>212</v>
       </c>
       <c r="E53" t="s">
         <v>12</v>
       </c>
       <c r="F53" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="H53" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="G53" s="2" t="s">
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>198</v>
+      </c>
+      <c r="B54" t="s">
+        <v>199</v>
+      </c>
+      <c r="C54" t="s">
+        <v>71</v>
+      </c>
+      <c r="D54" t="s">
         <v>214</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" t="s">
-        <v>200</v>
-      </c>
-      <c r="B54" t="s">
-        <v>201</v>
-      </c>
-      <c r="C54" t="s">
-        <v>73</v>
-      </c>
-      <c r="D54" t="s">
-        <v>216</v>
       </c>
       <c r="E54" t="s">
         <v>12</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G54" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>198</v>
+      </c>
+      <c r="B55" t="s">
+        <v>199</v>
+      </c>
+      <c r="C55" t="s">
+        <v>71</v>
+      </c>
+      <c r="D55" t="s">
         <v>217</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="E55" t="s">
+        <v>53</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" t="s">
-        <v>200</v>
-      </c>
-      <c r="B55" t="s">
-        <v>201</v>
-      </c>
-      <c r="C55" t="s">
-        <v>73</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="G55" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E55" t="s">
-        <v>55</v>
-      </c>
-      <c r="F55" s="2" t="s">
+      <c r="H55" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="G55" s="2" t="s">
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>198</v>
+      </c>
+      <c r="B56" t="s">
+        <v>199</v>
+      </c>
+      <c r="C56" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" t="s">
         <v>221</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="E56" t="s">
+        <v>48</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" t="s">
-        <v>200</v>
-      </c>
-      <c r="B56" t="s">
-        <v>201</v>
-      </c>
-      <c r="C56" t="s">
-        <v>73</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="G56" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="E56" t="s">
-        <v>50</v>
-      </c>
-      <c r="F56" s="2" t="s">
+      <c r="H56" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G56" s="2" t="s">
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>198</v>
+      </c>
+      <c r="B57" t="s">
+        <v>199</v>
+      </c>
+      <c r="C57" t="s">
+        <v>71</v>
+      </c>
+      <c r="D57" t="s">
         <v>225</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" t="s">
-        <v>200</v>
-      </c>
-      <c r="B57" t="s">
-        <v>201</v>
-      </c>
-      <c r="C57" t="s">
-        <v>73</v>
-      </c>
-      <c r="D57" t="s">
-        <v>227</v>
       </c>
       <c r="E57" t="s">
         <v>12</v>
       </c>
       <c r="F57" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="G57" s="2" t="s">
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>198</v>
+      </c>
+      <c r="B58" t="s">
+        <v>199</v>
+      </c>
+      <c r="C58" t="s">
+        <v>71</v>
+      </c>
+      <c r="D58" t="s">
         <v>229</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" t="s">
-        <v>200</v>
-      </c>
-      <c r="B58" t="s">
-        <v>201</v>
-      </c>
-      <c r="C58" t="s">
-        <v>73</v>
-      </c>
-      <c r="D58" t="s">
-        <v>231</v>
       </c>
       <c r="E58" t="s">
         <v>35</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -2689,22 +2681,22 @@
       <c r="G59" s="9"/>
       <c r="H59" s="4"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E61" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F61"/>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E62" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F62" s="16">
         <f>COUNTA(B2:B71)</f>
         <v>51</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E63" s="17" t="s">
         <v>8</v>
       </c>
@@ -2713,45 +2705,45 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E64" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F64" s="14">
         <f>COUNTIF(A2:A60, "Australia")</f>
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="5:6">
+    <row r="65" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E65" s="17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F65" s="14">
         <f>COUNTIF(A2:A60, "West Indian Ocean")</f>
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="5:6">
+    <row r="66" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E66" s="17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F66" s="14">
         <f>COUNTIF(A2:A60, "North Atlantic Ocean")</f>
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="5:6">
+    <row r="67" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E67" s="17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F67" s="14">
         <f>COUNTIF(A2:A60, "North Pacific Ocean")</f>
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="5:6">
+    <row r="68" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E68" s="17" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F68" s="14">
         <f>COUNTIF(A2:A60, "West Pacific Ocean")</f>

</xml_diff>

<commit_message>
added list of cyclones
</commit_message>
<xml_diff>
--- a/dataproc/list_of_cyclones.xlsx
+++ b/dataproc/list_of_cyclones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ren\forecast-diffmodels\dataproc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5494F137-A53E-4F5E-B04B-58C4C638C61D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD02CD5F-7991-412D-91C2-ED1C381434BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -727,10 +727,10 @@
     <t>South West Indian Ocean</t>
   </si>
   <si>
-    <t xml:space="preserve">28-10-2019	</t>
-  </si>
-  <si>
     <t>31-10-2019</t>
+  </si>
+  <si>
+    <t>28-10-2019</t>
   </si>
 </sst>
 </file>
@@ -1407,10 +1407,10 @@
         <v>35</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>36</v>

</xml_diff>